<commit_message>
added usage instructions to the README, updated names in sample narratives
</commit_message>
<xml_diff>
--- a/sample_narratives.xlsx
+++ b/sample_narratives.xlsx
@@ -61,7 +61,7 @@
     <t>Additional Comments?</t>
   </si>
   <si>
-    <t>Rob Ford</t>
+    <t>Ford, Rob</t>
   </si>
   <si>
     <t>male</t>
@@ -82,7 +82,7 @@
     <t>Good job</t>
   </si>
   <si>
-    <t>Frodo Baggins</t>
+    <t>Baggins, Frodo</t>
   </si>
   <si>
     <t>female</t>
@@ -110,7 +110,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -120,6 +120,16 @@
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Verdana"/>
     </font>
     <font>
       <sz val="10"/>
@@ -174,15 +184,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
   </cellXfs>

</xml_diff>